<commit_message>
Gestion des délégataires par communes
</commit_message>
<xml_diff>
--- a/static/files/communes.xlsx
+++ b/static/files/communes.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylvain/Projects/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17737C92-211D-0E40-B7CB-F791BE3FEF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDC12FF-5E70-464D-BCE9-AE2A8660AA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Financements" sheetId="1" r:id="rId1"/>
+    <sheet name="Communes" sheetId="1" r:id="rId1"/>
     <sheet name="Notice" sheetId="2" r:id="rId2"/>
     <sheet name="Data" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -842,7 +842,7 @@
   <dimension ref="B2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>